<commit_message>
update inclass data after 1_intro finished
</commit_message>
<xml_diff>
--- a/course_materials/Spring2019_inclass_schedule.xlsx
+++ b/course_materials/Spring2019_inclass_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfred/OneDrive - University of Nevada, Reno/Teaching/Bayes_course/git_public/course_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA72D174-A394-6245-A028-ED67B4F8B69B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A64388-3764-1B49-B8A5-DF66220B35A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21040" xr2:uid="{CC6B377C-2D53-2D4B-83BE-4520AEC28427}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34400" windowHeight="28260" xr2:uid="{CC6B377C-2D53-2D4B-83BE-4520AEC28427}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="11">
   <si>
     <t>Week</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Activity-based</t>
+  </si>
+  <si>
+    <t>See 1_intro.Rmd</t>
   </si>
 </sst>
 </file>
@@ -409,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F50BF90-29C5-6C4A-9EB5-01A0BD78BA62}">
   <dimension ref="A1:F128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,6 +442,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>43487</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>
@@ -451,8 +457,14 @@
       <c r="E2">
         <v>5</v>
       </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43487</v>
+      </c>
       <c r="B3">
         <v>1</v>
       </c>
@@ -467,6 +479,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43487</v>
+      </c>
       <c r="B4">
         <v>1</v>
       </c>
@@ -481,6 +496,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43487</v>
+      </c>
       <c r="B5">
         <v>1</v>
       </c>
@@ -491,10 +509,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43487</v>
+      </c>
       <c r="B6">
         <v>1</v>
       </c>
@@ -505,7 +526,7 @@
         <v>6</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>